<commit_message>
reducing the todo list
</commit_message>
<xml_diff>
--- a/Thesis/Documents/HashDistribution.xlsx
+++ b/Thesis/Documents/HashDistribution.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dany\Documents\Masterarbeit\dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\master-thesis\Thesis\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -125,7 +125,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>sha-256 </a:t>
+              <a:t>SHA256 </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2534,7 +2534,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
btc evaluation miner attack
</commit_message>
<xml_diff>
--- a/Thesis/Documents/HashDistribution.xlsx
+++ b/Thesis/Documents/HashDistribution.xlsx
@@ -2533,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>